<commit_message>
Updated and added new test cases.Removed outdated test cases
</commit_message>
<xml_diff>
--- a/TestCases/Test Case Template.xlsx
+++ b/TestCases/Test Case Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr/>
   <xr:revisionPtr revIDLastSave="241" documentId="73C46051A8BEC8499BD6F27A2EFF4919BEF0C8B8" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{A20FA539-5E42-43D2-902D-DBEE1F41A3D0}"/>
   <bookViews>
@@ -385,9 +385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>